<commit_message>
Aggiornamento file per accreditamento
Modifiche secondo quanto indicato nella mail di mancato accreditamento
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111SYNLABXXXXX/Synlab_SDN/Sdn.Net/1.1.0.0/accreditamento-checklist_V8.1.2.xlsx
+++ b/GATEWAY/A1#111SYNLABXXXXX/Synlab_SDN/Sdn.Net/1.1.0.0/accreditamento-checklist_V8.1.2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.1.163\D_Drive\tmp\RepositoryFSE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1051D49-3102-41DE-816F-5A4CFA91E0A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE32E53-FC34-4831-A689-5DD1A9DF13D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -23,8 +23,19 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestCases!$A$9:$T$374</definedName>
     <definedName name="filtro" localSheetId="2">TestCases!$A$9:$S$203</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataSignature="AMtx7mhUlYP9yzNmk4f07XMJovPPUaqOhw=="/>
     </ext>
@@ -4489,42 +4500,6 @@
     <t>subject_application_version: 1.1.0.0</t>
   </si>
   <si>
-    <t>2023-03-24T12:06:07Z</t>
-  </si>
-  <si>
-    <t>fa2efb37fdf61bb5</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.272c6c77018858a80bb1db201ec649fc871ad4df9bade202fb42c7162a72340e.b57c740d4f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-24T12:40:38Z</t>
-  </si>
-  <si>
-    <t>84d352d923837c4b</t>
-  </si>
-  <si>
-    <t>2023-03-24T12:47:46Z</t>
-  </si>
-  <si>
-    <t>4064f2331b3986d1</t>
-  </si>
-  <si>
-    <t>Campo token JWT non valido</t>
-  </si>
-  <si>
-    <t>Campo token JWT non valido. Il campo action_id non è corretto</t>
-  </si>
-  <si>
-    <t>2023-03-23T14:00:08Z</t>
-  </si>
-  <si>
-    <t>5e6901679234734e</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.6b949d13b8eb962b6a9d69668540a82cdaf5caa91b8df9dcc2fd6c98a49ce61e.bc5dd6ccae^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>L'errore di timeout è gestito dal software</t>
   </si>
   <si>
@@ -5173,15 +5148,6 @@
     <t>Aggiornamento non effettuato</t>
   </si>
   <si>
-    <t>2023-03-28T11:53:43Z</t>
-  </si>
-  <si>
-    <t>bc0b6bf2f2490c94</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.a1dac749a1137153a668f75288426a9ddbd840f6518b30cdd6c6c258cbb3449e.0eb3f62fcc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Il sistema non gestisce il campo "Storia Clinica","Accertamenti e controlli consigliati" nel referto</t>
   </si>
   <si>
@@ -5342,6 +5308,51 @@
   </si>
   <si>
     <t>Mancato Invio a FSE. Gestito in backoffice</t>
+  </si>
+  <si>
+    <t>2023-05-09T11:07:07Z</t>
+  </si>
+  <si>
+    <t>e298aeed926a2e8f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.f02e119ae90b94bc94c1cbcaa5ec8bd9a5328374bf30d14eb77eb2e852a9ee25.7ba745a11b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-05-09T11:17:28Z</t>
+  </si>
+  <si>
+    <t>c11b33a1d16382c9</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.bb5d2023458b0f49a993132451ba324414f01e3527713c570cb2a8d77b83bc46.399ef836be^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-05-09T11:21:48Z</t>
+  </si>
+  <si>
+    <t>24a23efe29eae750</t>
+  </si>
+  <si>
+    <t>Errore 403: Campo token JWT non valido</t>
+  </si>
+  <si>
+    <t>2023-05-09T11:26:15Z</t>
+  </si>
+  <si>
+    <t>709d23c09489b6c5</t>
+  </si>
+  <si>
+    <t>Errore 403: Campo token JWT non valido. Il campo action_id non è corretto</t>
+  </si>
+  <si>
+    <t>2023-05-09T11:32:23Z</t>
+  </si>
+  <si>
+    <t>0747b70516dae93a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.6b5a81c9c7d7f8e6a15b539e4cafd1878728df60a054218a5f5b866a20f46ad2.1c82bd6cc4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -8312,7 +8323,7 @@
   <dimension ref="A1:T992"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P223" sqref="P223"/>
+      <selection activeCell="I330" sqref="I330"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -8719,16 +8730,16 @@
         <v>424</v>
       </c>
       <c r="F14" s="26">
-        <v>45009</v>
+        <v>45055</v>
       </c>
       <c r="G14" s="27" t="s">
-        <v>833</v>
+        <v>1103</v>
       </c>
       <c r="H14" s="27" t="s">
-        <v>834</v>
+        <v>1104</v>
       </c>
       <c r="I14" s="27" t="s">
-        <v>835</v>
+        <v>1105</v>
       </c>
       <c r="J14" s="28" t="s">
         <v>488</v>
@@ -8769,16 +8780,16 @@
         <v>426</v>
       </c>
       <c r="F15" s="26">
-        <v>45009</v>
+        <v>45055</v>
       </c>
       <c r="G15" s="27" t="s">
-        <v>842</v>
+        <v>1106</v>
       </c>
       <c r="H15" s="27" t="s">
-        <v>843</v>
+        <v>1107</v>
       </c>
       <c r="I15" s="27" t="s">
-        <v>844</v>
+        <v>1108</v>
       </c>
       <c r="J15" s="28" t="s">
         <v>488</v>
@@ -8802,7 +8813,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="232.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:20" ht="247" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="23">
         <v>242</v>
       </c>
@@ -8836,7 +8847,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="218" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:20" ht="232.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="23">
         <v>253</v>
       </c>
@@ -8870,7 +8881,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="232.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:20" ht="247" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="23">
         <v>258</v>
       </c>
@@ -8904,7 +8915,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="218" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:20" ht="232.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="23">
         <v>269</v>
       </c>
@@ -9026,13 +9037,13 @@
         <v>45016</v>
       </c>
       <c r="G22" s="27" t="s">
-        <v>1050</v>
+        <v>1038</v>
       </c>
       <c r="H22" s="27" t="s">
-        <v>1049</v>
+        <v>1037</v>
       </c>
       <c r="I22" s="27" t="s">
-        <v>1051</v>
+        <v>1039</v>
       </c>
       <c r="J22" s="28" t="s">
         <v>488</v>
@@ -9076,13 +9087,13 @@
         <v>45016</v>
       </c>
       <c r="G23" s="27" t="s">
-        <v>1052</v>
+        <v>1040</v>
       </c>
       <c r="H23" s="27" t="s">
-        <v>1053</v>
+        <v>1041</v>
       </c>
       <c r="I23" s="27" t="s">
-        <v>860</v>
+        <v>848</v>
       </c>
       <c r="J23" s="28" t="s">
         <v>488</v>
@@ -9095,13 +9106,13 @@
         <v>488</v>
       </c>
       <c r="N23" s="28" t="s">
-        <v>929</v>
+        <v>917</v>
       </c>
       <c r="O23" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P23" s="28" t="s">
-        <v>1054</v>
+        <v>1042</v>
       </c>
       <c r="Q23" s="28" t="s">
         <v>826</v>
@@ -9340,7 +9351,7 @@
         <v>828</v>
       </c>
       <c r="K30" s="32" t="s">
-        <v>848</v>
+        <v>836</v>
       </c>
       <c r="L30" s="28"/>
       <c r="M30" s="28"/>
@@ -9378,7 +9389,7 @@
         <v>828</v>
       </c>
       <c r="K31" s="28" t="s">
-        <v>933</v>
+        <v>921</v>
       </c>
       <c r="L31" s="28"/>
       <c r="M31" s="28"/>
@@ -9392,7 +9403,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="174.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:20" ht="189" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="23">
         <v>358</v>
       </c>
@@ -9414,7 +9425,7 @@
       <c r="I32" s="27"/>
       <c r="J32" s="28"/>
       <c r="K32" s="33" t="s">
-        <v>846</v>
+        <v>834</v>
       </c>
       <c r="L32" s="28"/>
       <c r="M32" s="28"/>
@@ -9428,7 +9439,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="203.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:20" ht="218" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="23">
         <v>359</v>
       </c>
@@ -9450,7 +9461,7 @@
       <c r="I33" s="27"/>
       <c r="J33" s="28"/>
       <c r="K33" s="33" t="s">
-        <v>847</v>
+        <v>835</v>
       </c>
       <c r="L33" s="28"/>
       <c r="M33" s="28"/>
@@ -9464,7 +9475,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="174.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:20" ht="189" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="23">
         <v>360</v>
       </c>
@@ -9498,7 +9509,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="203.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:20" ht="218" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="23">
         <v>361</v>
       </c>
@@ -9620,13 +9631,13 @@
         <v>45033</v>
       </c>
       <c r="G38" s="27" t="s">
-        <v>1106</v>
+        <v>1091</v>
       </c>
       <c r="H38" s="34" t="s">
-        <v>1105</v>
+        <v>1090</v>
       </c>
       <c r="I38" s="27" t="s">
-        <v>860</v>
+        <v>848</v>
       </c>
       <c r="J38" s="28" t="s">
         <v>488</v>
@@ -9639,13 +9650,13 @@
         <v>828</v>
       </c>
       <c r="N38" s="28" t="s">
-        <v>1104</v>
+        <v>1089</v>
       </c>
       <c r="O38" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P38" s="28" t="s">
-        <v>1054</v>
+        <v>1042</v>
       </c>
       <c r="Q38" s="28" t="s">
         <v>826</v>
@@ -9676,13 +9687,13 @@
         <v>45022</v>
       </c>
       <c r="G39" s="27" t="s">
-        <v>1067</v>
+        <v>1052</v>
       </c>
       <c r="H39" s="27" t="s">
-        <v>1068</v>
+        <v>1053</v>
       </c>
       <c r="I39" s="27" t="s">
-        <v>860</v>
+        <v>848</v>
       </c>
       <c r="J39" s="28" t="s">
         <v>488</v>
@@ -9695,13 +9706,13 @@
         <v>488</v>
       </c>
       <c r="N39" s="28" t="s">
-        <v>1028</v>
+        <v>1016</v>
       </c>
       <c r="O39" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P39" s="28" t="s">
-        <v>1069</v>
+        <v>1054</v>
       </c>
       <c r="Q39" s="28" t="s">
         <v>826</v>
@@ -9814,7 +9825,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="116.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:20" ht="131" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="23">
         <v>204</v>
       </c>
@@ -9882,7 +9893,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="116.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:20" ht="131" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="23">
         <v>220</v>
       </c>
@@ -9933,16 +9944,16 @@
         <v>462</v>
       </c>
       <c r="F46" s="26">
-        <v>45009</v>
+        <v>45055</v>
       </c>
       <c r="G46" s="27" t="s">
-        <v>836</v>
+        <v>1109</v>
       </c>
       <c r="H46" s="27" t="s">
-        <v>837</v>
+        <v>1110</v>
       </c>
       <c r="I46" s="27" t="s">
-        <v>860</v>
+        <v>848</v>
       </c>
       <c r="J46" s="28" t="s">
         <v>488</v>
@@ -9955,13 +9966,13 @@
         <v>488</v>
       </c>
       <c r="N46" s="34" t="s">
-        <v>840</v>
+        <v>1111</v>
       </c>
       <c r="O46" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P46" s="28" t="s">
-        <v>1116</v>
+        <v>1101</v>
       </c>
       <c r="Q46" s="28" t="s">
         <v>826</v>
@@ -9989,16 +10000,16 @@
         <v>477</v>
       </c>
       <c r="F47" s="26">
-        <v>45009</v>
+        <v>45055</v>
       </c>
       <c r="G47" s="27" t="s">
-        <v>838</v>
+        <v>1112</v>
       </c>
       <c r="H47" s="27" t="s">
-        <v>839</v>
+        <v>1113</v>
       </c>
       <c r="I47" s="27" t="s">
-        <v>860</v>
+        <v>848</v>
       </c>
       <c r="J47" s="28" t="s">
         <v>488</v>
@@ -10011,13 +10022,13 @@
         <v>488</v>
       </c>
       <c r="N47" s="34" t="s">
-        <v>841</v>
+        <v>1114</v>
       </c>
       <c r="O47" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P47" s="28" t="s">
-        <v>1116</v>
+        <v>1101</v>
       </c>
       <c r="Q47" s="32" t="s">
         <v>826</v>
@@ -10062,7 +10073,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="116.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:20" ht="131" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="23">
         <v>252</v>
       </c>
@@ -10130,7 +10141,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="116.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:20" ht="131" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51" s="23">
         <v>268</v>
       </c>
@@ -10198,7 +10209,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="116.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:20" ht="131" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="23">
         <v>284</v>
       </c>
@@ -10252,13 +10263,13 @@
         <v>45016</v>
       </c>
       <c r="G54" s="27" t="s">
-        <v>1043</v>
+        <v>1031</v>
       </c>
       <c r="H54" s="27" t="s">
-        <v>1044</v>
+        <v>1032</v>
       </c>
       <c r="I54" s="27" t="s">
-        <v>1045</v>
+        <v>1033</v>
       </c>
       <c r="J54" s="28" t="s">
         <v>488</v>
@@ -10278,7 +10289,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="116.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:20" ht="131" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" s="23">
         <v>300</v>
       </c>
@@ -10298,13 +10309,13 @@
         <v>45016</v>
       </c>
       <c r="G55" s="27" t="s">
-        <v>1046</v>
+        <v>1034</v>
       </c>
       <c r="H55" s="27" t="s">
-        <v>1047</v>
+        <v>1035</v>
       </c>
       <c r="I55" s="27" t="s">
-        <v>860</v>
+        <v>848</v>
       </c>
       <c r="J55" s="28" t="s">
         <v>488</v>
@@ -10317,13 +10328,13 @@
         <v>488</v>
       </c>
       <c r="N55" s="28" t="s">
-        <v>929</v>
+        <v>917</v>
       </c>
       <c r="O55" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P55" s="28" t="s">
-        <v>1048</v>
+        <v>1036</v>
       </c>
       <c r="Q55" s="28" t="s">
         <v>826</v>
@@ -10368,7 +10379,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="116.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:20" ht="131" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A57" s="23">
         <v>316</v>
       </c>
@@ -10565,7 +10576,7 @@
       <c r="N62" s="28"/>
       <c r="O62" s="28"/>
       <c r="P62" s="32" t="s">
-        <v>845</v>
+        <v>833</v>
       </c>
       <c r="Q62" s="28"/>
       <c r="R62" s="29"/>
@@ -10594,13 +10605,13 @@
         <v>45009</v>
       </c>
       <c r="G63" s="35" t="s">
-        <v>855</v>
+        <v>843</v>
       </c>
       <c r="H63" s="27" t="s">
-        <v>849</v>
+        <v>837</v>
       </c>
       <c r="I63" s="27" t="s">
-        <v>859</v>
+        <v>847</v>
       </c>
       <c r="J63" s="32" t="s">
         <v>488</v>
@@ -10613,13 +10624,13 @@
         <v>488</v>
       </c>
       <c r="N63" s="32" t="s">
-        <v>850</v>
+        <v>838</v>
       </c>
       <c r="O63" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P63" s="28" t="s">
-        <v>1069</v>
+        <v>1054</v>
       </c>
       <c r="Q63" s="32" t="s">
         <v>826</v>
@@ -10854,13 +10865,13 @@
         <v>45016</v>
       </c>
       <c r="G70" s="27" t="s">
-        <v>1055</v>
+        <v>1043</v>
       </c>
       <c r="H70" s="27" t="s">
-        <v>1056</v>
+        <v>1044</v>
       </c>
       <c r="I70" s="27" t="s">
-        <v>1057</v>
+        <v>1045</v>
       </c>
       <c r="J70" s="28" t="s">
         <v>488</v>
@@ -10904,13 +10915,13 @@
         <v>45016</v>
       </c>
       <c r="G71" s="27" t="s">
-        <v>1058</v>
+        <v>1046</v>
       </c>
       <c r="H71" s="27" t="s">
-        <v>1059</v>
+        <v>1047</v>
       </c>
       <c r="I71" s="27" t="s">
-        <v>860</v>
+        <v>848</v>
       </c>
       <c r="J71" s="28" t="s">
         <v>488</v>
@@ -10923,13 +10934,13 @@
         <v>488</v>
       </c>
       <c r="N71" s="28" t="s">
-        <v>929</v>
+        <v>917</v>
       </c>
       <c r="O71" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P71" s="28" t="s">
-        <v>1060</v>
+        <v>1048</v>
       </c>
       <c r="Q71" s="28" t="s">
         <v>826</v>
@@ -11212,7 +11223,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="80" spans="1:20" ht="189" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:20" ht="203.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A80" s="23">
         <v>202</v>
       </c>
@@ -11280,7 +11291,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="82" spans="1:20" ht="160" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:20" ht="174.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A82" s="23">
         <v>208</v>
       </c>
@@ -11484,7 +11495,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="88" spans="1:20" ht="189" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:20" ht="203.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A88" s="23">
         <v>218</v>
       </c>
@@ -11572,13 +11583,13 @@
         <v>45009</v>
       </c>
       <c r="G90" s="35" t="s">
-        <v>854</v>
+        <v>842</v>
       </c>
       <c r="H90" s="27" t="s">
-        <v>851</v>
+        <v>839</v>
       </c>
       <c r="I90" s="27" t="s">
-        <v>858</v>
+        <v>846</v>
       </c>
       <c r="J90" s="32" t="s">
         <v>488</v>
@@ -11591,13 +11602,13 @@
         <v>488</v>
       </c>
       <c r="N90" s="32" t="s">
-        <v>852</v>
+        <v>840</v>
       </c>
       <c r="O90" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P90" s="28" t="s">
-        <v>1070</v>
+        <v>1055</v>
       </c>
       <c r="Q90" s="32" t="s">
         <v>826</v>
@@ -11608,7 +11619,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="91" spans="1:20" ht="160" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:20" ht="174.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A91" s="23">
         <v>77</v>
       </c>
@@ -11628,13 +11639,13 @@
         <v>45009</v>
       </c>
       <c r="G91" s="27" t="s">
-        <v>853</v>
+        <v>841</v>
       </c>
       <c r="H91" s="27" t="s">
-        <v>856</v>
+        <v>844</v>
       </c>
       <c r="I91" s="27" t="s">
-        <v>857</v>
+        <v>845</v>
       </c>
       <c r="J91" s="32" t="s">
         <v>488</v>
@@ -11647,13 +11658,13 @@
         <v>488</v>
       </c>
       <c r="N91" s="32" t="s">
-        <v>861</v>
+        <v>849</v>
       </c>
       <c r="O91" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P91" s="28" t="s">
-        <v>1070</v>
+        <v>1055</v>
       </c>
       <c r="Q91" s="32" t="s">
         <v>826</v>
@@ -11684,13 +11695,13 @@
         <v>45010</v>
       </c>
       <c r="G92" s="27" t="s">
-        <v>862</v>
+        <v>850</v>
       </c>
       <c r="H92" s="27" t="s">
-        <v>863</v>
+        <v>851</v>
       </c>
       <c r="I92" s="27" t="s">
-        <v>864</v>
+        <v>852</v>
       </c>
       <c r="J92" s="32" t="s">
         <v>488</v>
@@ -11703,13 +11714,13 @@
         <v>488</v>
       </c>
       <c r="N92" s="32" t="s">
-        <v>865</v>
+        <v>853</v>
       </c>
       <c r="O92" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P92" s="28" t="s">
-        <v>1070</v>
+        <v>1055</v>
       </c>
       <c r="Q92" s="32" t="s">
         <v>826</v>
@@ -11740,13 +11751,13 @@
         <v>45010</v>
       </c>
       <c r="G93" s="27" t="s">
-        <v>879</v>
+        <v>867</v>
       </c>
       <c r="H93" s="27" t="s">
-        <v>880</v>
+        <v>868</v>
       </c>
       <c r="I93" s="27" t="s">
-        <v>881</v>
+        <v>869</v>
       </c>
       <c r="J93" s="28" t="s">
         <v>488</v>
@@ -11759,13 +11770,13 @@
         <v>488</v>
       </c>
       <c r="N93" s="32" t="s">
-        <v>882</v>
+        <v>870</v>
       </c>
       <c r="O93" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P93" s="28" t="s">
-        <v>1070</v>
+        <v>1055</v>
       </c>
       <c r="Q93" s="32" t="s">
         <v>826</v>
@@ -11796,13 +11807,13 @@
         <v>45010</v>
       </c>
       <c r="G94" s="27" t="s">
-        <v>866</v>
+        <v>854</v>
       </c>
       <c r="H94" s="27" t="s">
-        <v>867</v>
+        <v>855</v>
       </c>
       <c r="I94" s="27" t="s">
-        <v>868</v>
+        <v>856</v>
       </c>
       <c r="J94" s="32" t="s">
         <v>488</v>
@@ -11815,13 +11826,13 @@
         <v>488</v>
       </c>
       <c r="N94" s="32" t="s">
-        <v>869</v>
+        <v>857</v>
       </c>
       <c r="O94" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P94" s="28" t="s">
-        <v>1070</v>
+        <v>1055</v>
       </c>
       <c r="Q94" s="32" t="s">
         <v>826</v>
@@ -11856,7 +11867,7 @@
         <v>828</v>
       </c>
       <c r="K95" s="32" t="s">
-        <v>870</v>
+        <v>858</v>
       </c>
       <c r="L95" s="28"/>
       <c r="M95" s="28"/>
@@ -11890,13 +11901,13 @@
         <v>45010</v>
       </c>
       <c r="G96" s="27" t="s">
-        <v>871</v>
+        <v>859</v>
       </c>
       <c r="H96" s="27" t="s">
-        <v>872</v>
+        <v>860</v>
       </c>
       <c r="I96" s="27" t="s">
-        <v>873</v>
+        <v>861</v>
       </c>
       <c r="J96" s="32" t="s">
         <v>488</v>
@@ -11909,13 +11920,13 @@
         <v>488</v>
       </c>
       <c r="N96" s="32" t="s">
-        <v>874</v>
+        <v>862</v>
       </c>
       <c r="O96" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P96" s="28" t="s">
-        <v>1070</v>
+        <v>1055</v>
       </c>
       <c r="Q96" s="32" t="s">
         <v>826</v>
@@ -11946,13 +11957,13 @@
         <v>45010</v>
       </c>
       <c r="G97" s="27" t="s">
-        <v>875</v>
+        <v>863</v>
       </c>
       <c r="H97" s="27" t="s">
-        <v>876</v>
+        <v>864</v>
       </c>
       <c r="I97" s="27" t="s">
-        <v>877</v>
+        <v>865</v>
       </c>
       <c r="J97" s="32" t="s">
         <v>488</v>
@@ -11965,13 +11976,13 @@
         <v>488</v>
       </c>
       <c r="N97" s="32" t="s">
-        <v>878</v>
+        <v>866</v>
       </c>
       <c r="O97" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P97" s="28" t="s">
-        <v>1070</v>
+        <v>1055</v>
       </c>
       <c r="Q97" s="32" t="s">
         <v>826</v>
@@ -12186,7 +12197,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="104" spans="1:20" ht="203.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:20" ht="218" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A104" s="23">
         <v>250</v>
       </c>
@@ -12458,7 +12469,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="112" spans="1:20" ht="203.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:20" ht="218" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A112" s="23">
         <v>266</v>
       </c>
@@ -12730,7 +12741,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="120" spans="1:20" ht="189" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:20" ht="203.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A120" s="23">
         <v>282</v>
       </c>
@@ -12798,7 +12809,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="122" spans="1:20" ht="160" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="122" spans="1:20" ht="174.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A122" s="23">
         <v>288</v>
       </c>
@@ -12818,13 +12829,13 @@
         <v>45014</v>
       </c>
       <c r="G122" s="27" t="s">
-        <v>997</v>
+        <v>985</v>
       </c>
       <c r="H122" s="27" t="s">
-        <v>998</v>
+        <v>986</v>
       </c>
       <c r="I122" s="27" t="s">
-        <v>999</v>
+        <v>987</v>
       </c>
       <c r="J122" s="28" t="s">
         <v>488</v>
@@ -12868,13 +12879,13 @@
         <v>45014</v>
       </c>
       <c r="G123" s="27" t="s">
-        <v>1000</v>
+        <v>988</v>
       </c>
       <c r="H123" s="27" t="s">
-        <v>1001</v>
+        <v>989</v>
       </c>
       <c r="I123" s="27" t="s">
-        <v>860</v>
+        <v>848</v>
       </c>
       <c r="J123" s="28" t="s">
         <v>488</v>
@@ -12887,13 +12898,13 @@
         <v>488</v>
       </c>
       <c r="N123" s="28" t="s">
-        <v>1002</v>
+        <v>990</v>
       </c>
       <c r="O123" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P123" s="28" t="s">
-        <v>1003</v>
+        <v>991</v>
       </c>
       <c r="Q123" s="28" t="s">
         <v>826</v>
@@ -12924,13 +12935,13 @@
         <v>45014</v>
       </c>
       <c r="G124" s="27" t="s">
-        <v>1004</v>
+        <v>992</v>
       </c>
       <c r="H124" s="27" t="s">
-        <v>1005</v>
+        <v>993</v>
       </c>
       <c r="I124" s="27" t="s">
-        <v>860</v>
+        <v>848</v>
       </c>
       <c r="J124" s="28" t="s">
         <v>488</v>
@@ -12943,13 +12954,13 @@
         <v>488</v>
       </c>
       <c r="N124" s="28" t="s">
-        <v>1006</v>
+        <v>994</v>
       </c>
       <c r="O124" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P124" s="28" t="s">
-        <v>1003</v>
+        <v>991</v>
       </c>
       <c r="Q124" s="28" t="s">
         <v>826</v>
@@ -12980,13 +12991,13 @@
         <v>45014</v>
       </c>
       <c r="G125" s="27" t="s">
-        <v>1007</v>
+        <v>995</v>
       </c>
       <c r="H125" s="27" t="s">
-        <v>1008</v>
+        <v>996</v>
       </c>
       <c r="I125" s="27" t="s">
-        <v>1009</v>
+        <v>997</v>
       </c>
       <c r="J125" s="28" t="s">
         <v>488</v>
@@ -13003,7 +13014,7 @@
         <v>828</v>
       </c>
       <c r="P125" s="28" t="s">
-        <v>1094</v>
+        <v>1079</v>
       </c>
       <c r="Q125" s="28" t="s">
         <v>826</v>
@@ -13034,13 +13045,13 @@
         <v>45014</v>
       </c>
       <c r="G126" s="27" t="s">
-        <v>1010</v>
+        <v>998</v>
       </c>
       <c r="H126" s="27" t="s">
-        <v>1011</v>
+        <v>999</v>
       </c>
       <c r="I126" s="27" t="s">
-        <v>860</v>
+        <v>848</v>
       </c>
       <c r="J126" s="28" t="s">
         <v>488</v>
@@ -13053,13 +13064,13 @@
         <v>488</v>
       </c>
       <c r="N126" s="28" t="s">
-        <v>1012</v>
+        <v>1000</v>
       </c>
       <c r="O126" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P126" s="28" t="s">
-        <v>1013</v>
+        <v>1001</v>
       </c>
       <c r="Q126" s="28" t="s">
         <v>826</v>
@@ -13090,13 +13101,13 @@
         <v>45014</v>
       </c>
       <c r="G127" s="27" t="s">
-        <v>1014</v>
+        <v>1002</v>
       </c>
       <c r="H127" s="27" t="s">
-        <v>1015</v>
+        <v>1003</v>
       </c>
       <c r="I127" s="27" t="s">
-        <v>1016</v>
+        <v>1004</v>
       </c>
       <c r="J127" s="28" t="s">
         <v>488</v>
@@ -13109,13 +13120,13 @@
         <v>828</v>
       </c>
       <c r="N127" s="28" t="s">
-        <v>1095</v>
+        <v>1080</v>
       </c>
       <c r="O127" s="28" t="s">
         <v>828</v>
       </c>
       <c r="P127" s="28" t="s">
-        <v>1096</v>
+        <v>1081</v>
       </c>
       <c r="Q127" s="28" t="s">
         <v>826</v>
@@ -13126,7 +13137,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="128" spans="1:20" ht="189" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="128" spans="1:20" ht="203.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A128" s="23">
         <v>298</v>
       </c>
@@ -13146,13 +13157,13 @@
         <v>45014</v>
       </c>
       <c r="G128" s="27" t="s">
-        <v>1017</v>
+        <v>1005</v>
       </c>
       <c r="H128" s="27" t="s">
-        <v>1018</v>
+        <v>1006</v>
       </c>
       <c r="I128" s="27" t="s">
-        <v>1019</v>
+        <v>1007</v>
       </c>
       <c r="J128" s="28" t="s">
         <v>488</v>
@@ -13165,13 +13176,13 @@
         <v>828</v>
       </c>
       <c r="N128" s="44" t="s">
-        <v>1097</v>
+        <v>1082</v>
       </c>
       <c r="O128" s="28" t="s">
         <v>828</v>
       </c>
       <c r="P128" s="28" t="s">
-        <v>1069</v>
+        <v>1054</v>
       </c>
       <c r="Q128" s="28" t="s">
         <v>826</v>
@@ -13202,13 +13213,13 @@
         <v>45014</v>
       </c>
       <c r="G129" s="27" t="s">
-        <v>1020</v>
+        <v>1008</v>
       </c>
       <c r="H129" s="27" t="s">
-        <v>1021</v>
+        <v>1009</v>
       </c>
       <c r="I129" s="27" t="s">
-        <v>1022</v>
+        <v>1010</v>
       </c>
       <c r="J129" s="28" t="s">
         <v>488</v>
@@ -13221,13 +13232,13 @@
         <v>828</v>
       </c>
       <c r="N129" s="28" t="s">
-        <v>1097</v>
+        <v>1082</v>
       </c>
       <c r="O129" s="28" t="s">
         <v>828</v>
       </c>
       <c r="P129" s="28" t="s">
-        <v>1069</v>
+        <v>1054</v>
       </c>
       <c r="Q129" s="28" t="s">
         <v>826</v>
@@ -13442,7 +13453,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="136" spans="1:20" ht="189" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="136" spans="1:20" ht="203.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A136" s="23">
         <v>314</v>
       </c>
@@ -13666,13 +13677,13 @@
         <v>45010</v>
       </c>
       <c r="G142" s="27" t="s">
-        <v>883</v>
+        <v>871</v>
       </c>
       <c r="H142" s="27" t="s">
-        <v>884</v>
+        <v>872</v>
       </c>
       <c r="I142" s="27" t="s">
-        <v>885</v>
+        <v>873</v>
       </c>
       <c r="J142" s="32" t="s">
         <v>488</v>
@@ -13685,13 +13696,13 @@
         <v>488</v>
       </c>
       <c r="N142" s="32" t="s">
-        <v>882</v>
+        <v>870</v>
       </c>
       <c r="O142" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P142" s="28" t="s">
-        <v>1071</v>
+        <v>1056</v>
       </c>
       <c r="Q142" s="32" t="s">
         <v>826</v>
@@ -13722,13 +13733,13 @@
         <v>45010</v>
       </c>
       <c r="G143" s="27" t="s">
-        <v>886</v>
+        <v>874</v>
       </c>
       <c r="H143" s="27" t="s">
-        <v>887</v>
+        <v>875</v>
       </c>
       <c r="I143" s="27" t="s">
-        <v>888</v>
+        <v>876</v>
       </c>
       <c r="J143" s="28" t="s">
         <v>488</v>
@@ -13741,13 +13752,13 @@
         <v>488</v>
       </c>
       <c r="N143" s="32" t="s">
-        <v>889</v>
+        <v>877</v>
       </c>
       <c r="O143" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P143" s="28" t="s">
-        <v>1071</v>
+        <v>1056</v>
       </c>
       <c r="Q143" s="32" t="s">
         <v>826</v>
@@ -13982,13 +13993,13 @@
         <v>45014</v>
       </c>
       <c r="G150" s="27" t="s">
-        <v>1023</v>
+        <v>1011</v>
       </c>
       <c r="H150" s="27" t="s">
-        <v>1024</v>
+        <v>1012</v>
       </c>
       <c r="I150" s="27" t="s">
-        <v>860</v>
+        <v>848</v>
       </c>
       <c r="J150" s="28" t="s">
         <v>488</v>
@@ -14001,13 +14012,13 @@
         <v>488</v>
       </c>
       <c r="N150" s="28" t="s">
-        <v>1025</v>
+        <v>1013</v>
       </c>
       <c r="O150" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P150" s="28" t="s">
-        <v>1003</v>
+        <v>991</v>
       </c>
       <c r="Q150" s="28" t="s">
         <v>826</v>
@@ -14038,13 +14049,13 @@
         <v>45014</v>
       </c>
       <c r="G151" s="27" t="s">
-        <v>1026</v>
+        <v>1014</v>
       </c>
       <c r="H151" s="27" t="s">
-        <v>1027</v>
+        <v>1015</v>
       </c>
       <c r="I151" s="27" t="s">
-        <v>860</v>
+        <v>848</v>
       </c>
       <c r="J151" s="28" t="s">
         <v>488</v>
@@ -14057,13 +14068,13 @@
         <v>488</v>
       </c>
       <c r="N151" s="28" t="s">
-        <v>1028</v>
+        <v>1016</v>
       </c>
       <c r="O151" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P151" s="28" t="s">
-        <v>1003</v>
+        <v>991</v>
       </c>
       <c r="Q151" s="28" t="s">
         <v>826</v>
@@ -14142,7 +14153,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="154" spans="1:20" ht="247" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="154" spans="1:20" ht="261.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A154" s="23">
         <v>193</v>
       </c>
@@ -14176,7 +14187,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="155" spans="1:20" ht="247" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="155" spans="1:20" ht="276" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A155" s="23">
         <v>206</v>
       </c>
@@ -14210,7 +14221,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="156" spans="1:20" ht="247" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="156" spans="1:20" ht="261.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A156" s="23">
         <v>209</v>
       </c>
@@ -14244,7 +14255,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="157" spans="1:20" ht="232.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="157" spans="1:20" ht="261.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A157" s="23">
         <v>222</v>
       </c>
@@ -14302,7 +14313,7 @@
         <v>828</v>
       </c>
       <c r="K158" s="32" t="s">
-        <v>890</v>
+        <v>878</v>
       </c>
       <c r="L158" s="28"/>
       <c r="M158" s="28"/>
@@ -14340,7 +14351,7 @@
         <v>828</v>
       </c>
       <c r="K159" s="32" t="s">
-        <v>891</v>
+        <v>879</v>
       </c>
       <c r="L159" s="28"/>
       <c r="M159" s="28"/>
@@ -14354,7 +14365,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="160" spans="1:20" ht="261.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="160" spans="1:20" ht="290.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A160" s="23">
         <v>241</v>
       </c>
@@ -14388,7 +14399,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="161" spans="1:20" ht="247" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="161" spans="1:20" ht="276" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A161" s="23">
         <v>254</v>
       </c>
@@ -14422,7 +14433,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="162" spans="1:20" ht="261.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="162" spans="1:20" ht="290.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A162" s="23">
         <v>257</v>
       </c>
@@ -14456,7 +14467,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="163" spans="1:20" ht="247" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="163" spans="1:20" ht="276" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A163" s="23">
         <v>270</v>
       </c>
@@ -14490,7 +14501,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="164" spans="1:20" ht="247" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="164" spans="1:20" ht="261.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A164" s="23">
         <v>273</v>
       </c>
@@ -14524,7 +14535,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="165" spans="1:20" ht="232.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="165" spans="1:20" ht="261.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A165" s="23">
         <v>286</v>
       </c>
@@ -14558,7 +14569,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="166" spans="1:20" ht="247" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="166" spans="1:20" ht="261.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A166" s="23">
         <v>289</v>
       </c>
@@ -14578,13 +14589,13 @@
         <v>45014</v>
       </c>
       <c r="G166" s="27" t="s">
-        <v>1029</v>
+        <v>1017</v>
       </c>
       <c r="H166" s="27" t="s">
-        <v>1030</v>
+        <v>1018</v>
       </c>
       <c r="I166" s="27" t="s">
-        <v>1031</v>
+        <v>1019</v>
       </c>
       <c r="J166" s="28" t="s">
         <v>488</v>
@@ -14604,13 +14615,13 @@
       </c>
       <c r="R166" s="29"/>
       <c r="S166" s="30" t="s">
-        <v>1032</v>
+        <v>1020</v>
       </c>
       <c r="T166" s="31" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="167" spans="1:20" ht="232.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="167" spans="1:20" ht="261.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A167" s="23">
         <v>302</v>
       </c>
@@ -14630,13 +14641,13 @@
         <v>45035</v>
       </c>
       <c r="G167" s="27" t="s">
-        <v>1113</v>
+        <v>1098</v>
       </c>
       <c r="H167" s="27" t="s">
-        <v>1114</v>
+        <v>1099</v>
       </c>
       <c r="I167" s="27" t="s">
-        <v>860</v>
+        <v>848</v>
       </c>
       <c r="J167" s="28" t="s">
         <v>488</v>
@@ -14649,13 +14660,13 @@
         <v>488</v>
       </c>
       <c r="N167" s="28" t="s">
-        <v>1115</v>
+        <v>1100</v>
       </c>
       <c r="O167" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P167" s="28" t="s">
-        <v>1116</v>
+        <v>1101</v>
       </c>
       <c r="Q167" s="28" t="s">
         <v>826</v>
@@ -14666,7 +14677,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="168" spans="1:20" ht="247" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="168" spans="1:20" ht="261.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A168" s="23">
         <v>305</v>
       </c>
@@ -14700,7 +14711,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="169" spans="1:20" ht="232.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="169" spans="1:20" ht="261.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A169" s="23">
         <v>318</v>
       </c>
@@ -14734,7 +14745,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="170" spans="1:20" ht="189" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="170" spans="1:20" ht="203.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A170" s="23">
         <v>322</v>
       </c>
@@ -14768,7 +14779,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="171" spans="1:20" ht="218" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="171" spans="1:20" ht="232.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A171" s="23">
         <v>323</v>
       </c>
@@ -14802,7 +14813,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="172" spans="1:20" ht="189" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="172" spans="1:20" ht="203.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A172" s="23">
         <v>326</v>
       </c>
@@ -14836,7 +14847,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="173" spans="1:20" ht="218" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="173" spans="1:20" ht="232.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A173" s="23">
         <v>327</v>
       </c>
@@ -14894,7 +14905,7 @@
         <v>828</v>
       </c>
       <c r="K174" s="32" t="s">
-        <v>892</v>
+        <v>880</v>
       </c>
       <c r="L174" s="28"/>
       <c r="M174" s="28"/>
@@ -14932,7 +14943,7 @@
         <v>828</v>
       </c>
       <c r="K175" s="28" t="s">
-        <v>934</v>
+        <v>922</v>
       </c>
       <c r="L175" s="28"/>
       <c r="M175" s="28"/>
@@ -14946,7 +14957,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="176" spans="1:20" ht="189" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="176" spans="1:20" ht="203.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A176" s="23">
         <v>334</v>
       </c>
@@ -14980,7 +14991,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="177" spans="1:20" ht="232.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="177" spans="1:20" ht="247" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A177" s="23">
         <v>335</v>
       </c>
@@ -15014,7 +15025,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="178" spans="1:20" ht="203.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="178" spans="1:20" ht="218" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A178" s="23">
         <v>338</v>
       </c>
@@ -15048,7 +15059,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="179" spans="1:20" ht="232.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="179" spans="1:20" ht="247" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A179" s="23">
         <v>339</v>
       </c>
@@ -15082,7 +15093,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="180" spans="1:20" ht="189" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="180" spans="1:20" ht="203.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A180" s="23">
         <v>342</v>
       </c>
@@ -15116,7 +15127,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="181" spans="1:20" ht="218" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="181" spans="1:20" ht="232.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A181" s="23">
         <v>343</v>
       </c>
@@ -15150,7 +15161,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="182" spans="1:20" ht="174.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="182" spans="1:20" ht="189" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A182" s="23">
         <v>346</v>
       </c>
@@ -15170,13 +15181,13 @@
         <v>45033</v>
       </c>
       <c r="G182" s="27" t="s">
-        <v>1108</v>
+        <v>1093</v>
       </c>
       <c r="H182" s="34" t="s">
-        <v>1107</v>
+        <v>1092</v>
       </c>
       <c r="I182" s="27" t="s">
-        <v>860</v>
+        <v>848</v>
       </c>
       <c r="J182" s="28" t="s">
         <v>488</v>
@@ -15189,13 +15200,13 @@
         <v>488</v>
       </c>
       <c r="N182" s="28" t="s">
-        <v>1109</v>
+        <v>1094</v>
       </c>
       <c r="O182" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P182" s="28" t="s">
-        <v>1033</v>
+        <v>1021</v>
       </c>
       <c r="Q182" s="28" t="s">
         <v>826</v>
@@ -15206,7 +15217,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="183" spans="1:20" ht="218" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="183" spans="1:20" ht="232.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A183" s="23">
         <v>347</v>
       </c>
@@ -15226,13 +15237,13 @@
         <v>45014</v>
       </c>
       <c r="G183" s="27" t="s">
-        <v>1034</v>
+        <v>1022</v>
       </c>
       <c r="H183" s="27" t="s">
-        <v>1035</v>
+        <v>1023</v>
       </c>
       <c r="I183" s="27" t="s">
-        <v>860</v>
+        <v>848</v>
       </c>
       <c r="J183" s="28" t="s">
         <v>488</v>
@@ -15245,26 +15256,26 @@
         <v>488</v>
       </c>
       <c r="N183" s="28" t="s">
-        <v>1028</v>
+        <v>1016</v>
       </c>
       <c r="O183" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P183" s="28" t="s">
-        <v>1033</v>
+        <v>1021</v>
       </c>
       <c r="Q183" s="28" t="s">
         <v>826</v>
       </c>
       <c r="R183" s="29"/>
       <c r="S183" s="30" t="s">
-        <v>1036</v>
+        <v>1024</v>
       </c>
       <c r="T183" s="31" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="184" spans="1:20" ht="189" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="184" spans="1:20" ht="203.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A184" s="23">
         <v>350</v>
       </c>
@@ -15298,7 +15309,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="185" spans="1:20" ht="218" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="185" spans="1:20" ht="232.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A185" s="23">
         <v>351</v>
       </c>
@@ -15662,7 +15673,7 @@
         <v>828</v>
       </c>
       <c r="K195" s="32" t="s">
-        <v>893</v>
+        <v>881</v>
       </c>
       <c r="L195" s="28"/>
       <c r="M195" s="28"/>
@@ -15700,7 +15711,7 @@
         <v>828</v>
       </c>
       <c r="K196" s="28" t="s">
-        <v>934</v>
+        <v>922</v>
       </c>
       <c r="L196" s="28"/>
       <c r="M196" s="28"/>
@@ -15734,13 +15745,13 @@
         <v>45012</v>
       </c>
       <c r="G197" s="27" t="s">
-        <v>894</v>
+        <v>882</v>
       </c>
       <c r="H197" s="27" t="s">
-        <v>895</v>
+        <v>883</v>
       </c>
       <c r="I197" s="27" t="s">
-        <v>896</v>
+        <v>884</v>
       </c>
       <c r="J197" s="28" t="s">
         <v>488</v>
@@ -15753,13 +15764,13 @@
         <v>488</v>
       </c>
       <c r="N197" s="32" t="s">
-        <v>897</v>
+        <v>885</v>
       </c>
       <c r="O197" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P197" s="28" t="s">
-        <v>1072</v>
+        <v>1057</v>
       </c>
       <c r="Q197" s="28" t="s">
         <v>826</v>
@@ -15790,13 +15801,13 @@
         <v>45012</v>
       </c>
       <c r="G198" s="27" t="s">
-        <v>898</v>
+        <v>886</v>
       </c>
       <c r="H198" s="27" t="s">
-        <v>899</v>
+        <v>887</v>
       </c>
       <c r="I198" s="27" t="s">
-        <v>900</v>
+        <v>888</v>
       </c>
       <c r="J198" s="28" t="s">
         <v>488</v>
@@ -15809,13 +15820,13 @@
         <v>488</v>
       </c>
       <c r="N198" s="32" t="s">
-        <v>901</v>
+        <v>889</v>
       </c>
       <c r="O198" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P198" s="28" t="s">
-        <v>1072</v>
+        <v>1057</v>
       </c>
       <c r="Q198" s="28" t="s">
         <v>826</v>
@@ -16336,7 +16347,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="214" spans="1:20" ht="160" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="214" spans="1:20" ht="174.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A214" s="23">
         <v>224</v>
       </c>
@@ -16356,13 +16367,13 @@
         <v>45012</v>
       </c>
       <c r="G214" s="27" t="s">
-        <v>902</v>
+        <v>890</v>
       </c>
       <c r="H214" s="37" t="s">
-        <v>903</v>
+        <v>891</v>
       </c>
       <c r="I214" s="27" t="s">
-        <v>904</v>
+        <v>892</v>
       </c>
       <c r="J214" s="28" t="s">
         <v>488</v>
@@ -16406,13 +16417,13 @@
         <v>45015</v>
       </c>
       <c r="G215" s="27" t="s">
-        <v>1037</v>
+        <v>1025</v>
       </c>
       <c r="H215" s="27" t="s">
-        <v>1038</v>
+        <v>1026</v>
       </c>
       <c r="I215" s="27" t="s">
-        <v>860</v>
+        <v>848</v>
       </c>
       <c r="J215" s="28" t="s">
         <v>488</v>
@@ -16425,13 +16436,13 @@
         <v>488</v>
       </c>
       <c r="N215" s="26" t="s">
-        <v>1039</v>
+        <v>1027</v>
       </c>
       <c r="O215" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P215" s="28" t="s">
-        <v>1117</v>
+        <v>1102</v>
       </c>
       <c r="Q215" s="28" t="s">
         <v>826</v>
@@ -16646,7 +16657,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="222" spans="1:20" ht="247" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="222" spans="1:20" ht="261.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A222" s="23">
         <v>225</v>
       </c>
@@ -16666,13 +16677,13 @@
         <v>45012</v>
       </c>
       <c r="G222" s="27" t="s">
-        <v>905</v>
+        <v>893</v>
       </c>
       <c r="H222" s="27" t="s">
-        <v>906</v>
+        <v>894</v>
       </c>
       <c r="I222" s="27" t="s">
-        <v>907</v>
+        <v>895</v>
       </c>
       <c r="J222" s="28" t="s">
         <v>488</v>
@@ -16716,13 +16727,13 @@
         <v>45015</v>
       </c>
       <c r="G223" s="27" t="s">
-        <v>1040</v>
+        <v>1028</v>
       </c>
       <c r="H223" s="27" t="s">
-        <v>1041</v>
+        <v>1029</v>
       </c>
       <c r="I223" s="27" t="s">
-        <v>860</v>
+        <v>848</v>
       </c>
       <c r="J223" s="28" t="s">
         <v>488</v>
@@ -16735,13 +16746,13 @@
         <v>488</v>
       </c>
       <c r="N223" s="28" t="s">
-        <v>1042</v>
+        <v>1030</v>
       </c>
       <c r="O223" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P223" s="28" t="s">
-        <v>1117</v>
+        <v>1102</v>
       </c>
       <c r="Q223" s="28" t="s">
         <v>826</v>
@@ -16982,13 +16993,13 @@
         <v>45022</v>
       </c>
       <c r="G230" s="27" t="s">
-        <v>1073</v>
+        <v>1058</v>
       </c>
       <c r="H230" s="34" t="s">
-        <v>1074</v>
+        <v>1059</v>
       </c>
       <c r="I230" s="34" t="s">
-        <v>1075</v>
+        <v>1060</v>
       </c>
       <c r="J230" s="28" t="s">
         <v>488</v>
@@ -17040,7 +17051,7 @@
       <c r="N231" s="28"/>
       <c r="O231" s="28"/>
       <c r="P231" s="28" t="s">
-        <v>1076</v>
+        <v>1061</v>
       </c>
       <c r="Q231" s="28" t="s">
         <v>826</v>
@@ -17961,13 +17972,13 @@
         <v>45012</v>
       </c>
       <c r="G258" s="27" t="s">
-        <v>908</v>
+        <v>896</v>
       </c>
       <c r="H258" s="27" t="s">
-        <v>909</v>
+        <v>897</v>
       </c>
       <c r="I258" s="27" t="s">
-        <v>910</v>
+        <v>898</v>
       </c>
       <c r="J258" s="28" t="s">
         <v>488</v>
@@ -18011,13 +18022,13 @@
         <v>45013</v>
       </c>
       <c r="G259" s="27" t="s">
-        <v>935</v>
+        <v>923</v>
       </c>
       <c r="H259" s="27" t="s">
-        <v>936</v>
+        <v>924</v>
       </c>
       <c r="I259" s="27" t="s">
-        <v>937</v>
+        <v>925</v>
       </c>
       <c r="J259" s="28" t="s">
         <v>488</v>
@@ -18061,13 +18072,13 @@
         <v>45012</v>
       </c>
       <c r="G260" s="27" t="s">
-        <v>911</v>
+        <v>899</v>
       </c>
       <c r="H260" s="34" t="s">
-        <v>912</v>
+        <v>900</v>
       </c>
       <c r="I260" s="27" t="s">
-        <v>860</v>
+        <v>848</v>
       </c>
       <c r="J260" s="28" t="s">
         <v>488</v>
@@ -18080,13 +18091,13 @@
         <v>488</v>
       </c>
       <c r="N260" s="34" t="s">
-        <v>913</v>
+        <v>901</v>
       </c>
       <c r="O260" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P260" s="28" t="s">
-        <v>1072</v>
+        <v>1057</v>
       </c>
       <c r="Q260" s="28" t="s">
         <v>826</v>
@@ -18117,13 +18128,13 @@
         <v>45012</v>
       </c>
       <c r="G261" s="27" t="s">
-        <v>914</v>
+        <v>902</v>
       </c>
       <c r="H261" s="27" t="s">
-        <v>915</v>
+        <v>903</v>
       </c>
       <c r="I261" s="27" t="s">
-        <v>860</v>
+        <v>848</v>
       </c>
       <c r="J261" s="28" t="s">
         <v>488</v>
@@ -18136,13 +18147,13 @@
         <v>488</v>
       </c>
       <c r="N261" s="28" t="s">
-        <v>1077</v>
+        <v>1062</v>
       </c>
       <c r="O261" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P261" s="28" t="s">
-        <v>1078</v>
+        <v>1063</v>
       </c>
       <c r="Q261" s="28" t="s">
         <v>826</v>
@@ -18173,13 +18184,13 @@
         <v>45012</v>
       </c>
       <c r="G262" s="27" t="s">
-        <v>916</v>
+        <v>904</v>
       </c>
       <c r="H262" s="27" t="s">
-        <v>917</v>
+        <v>905</v>
       </c>
       <c r="I262" s="27" t="s">
-        <v>918</v>
+        <v>906</v>
       </c>
       <c r="J262" s="28" t="s">
         <v>488</v>
@@ -18192,20 +18203,20 @@
         <v>828</v>
       </c>
       <c r="N262" s="28" t="s">
-        <v>1098</v>
+        <v>1083</v>
       </c>
       <c r="O262" s="28" t="s">
         <v>828</v>
       </c>
       <c r="P262" s="28" t="s">
-        <v>1098</v>
+        <v>1083</v>
       </c>
       <c r="Q262" s="28" t="s">
         <v>826</v>
       </c>
       <c r="R262" s="29"/>
       <c r="S262" s="38" t="s">
-        <v>919</v>
+        <v>907</v>
       </c>
       <c r="T262" s="31" t="s">
         <v>51</v>
@@ -18231,13 +18242,13 @@
         <v>45012</v>
       </c>
       <c r="G263" s="27" t="s">
-        <v>920</v>
+        <v>908</v>
       </c>
       <c r="H263" s="27" t="s">
-        <v>921</v>
+        <v>909</v>
       </c>
       <c r="I263" s="27" t="s">
-        <v>860</v>
+        <v>848</v>
       </c>
       <c r="J263" s="28" t="s">
         <v>488</v>
@@ -18250,13 +18261,13 @@
         <v>488</v>
       </c>
       <c r="N263" s="32" t="s">
-        <v>922</v>
+        <v>910</v>
       </c>
       <c r="O263" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P263" s="28" t="s">
-        <v>1079</v>
+        <v>1064</v>
       </c>
       <c r="Q263" s="28" t="s">
         <v>826</v>
@@ -18287,13 +18298,13 @@
         <v>45012</v>
       </c>
       <c r="G264" s="27" t="s">
-        <v>923</v>
+        <v>911</v>
       </c>
       <c r="H264" s="27" t="s">
-        <v>927</v>
+        <v>915</v>
       </c>
       <c r="I264" s="27" t="s">
-        <v>924</v>
+        <v>912</v>
       </c>
       <c r="J264" s="28" t="s">
         <v>488</v>
@@ -18306,26 +18317,26 @@
         <v>828</v>
       </c>
       <c r="N264" s="28" t="s">
-        <v>1098</v>
+        <v>1083</v>
       </c>
       <c r="O264" s="28" t="s">
         <v>828</v>
       </c>
       <c r="P264" s="28" t="s">
-        <v>1099</v>
+        <v>1084</v>
       </c>
       <c r="Q264" s="28" t="s">
         <v>826</v>
       </c>
       <c r="R264" s="29"/>
       <c r="S264" s="38" t="s">
-        <v>925</v>
+        <v>913</v>
       </c>
       <c r="T264" s="31" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="265" spans="1:20" ht="189" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="265" spans="1:20" ht="203.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A265" s="23">
         <v>234</v>
       </c>
@@ -18345,13 +18356,13 @@
         <v>45013</v>
       </c>
       <c r="G265" s="27" t="s">
-        <v>938</v>
+        <v>926</v>
       </c>
       <c r="H265" s="27" t="s">
-        <v>939</v>
+        <v>927</v>
       </c>
       <c r="I265" s="27" t="s">
-        <v>940</v>
+        <v>928</v>
       </c>
       <c r="J265" s="28" t="s">
         <v>488</v>
@@ -18364,20 +18375,20 @@
         <v>828</v>
       </c>
       <c r="N265" s="28" t="s">
-        <v>1098</v>
+        <v>1083</v>
       </c>
       <c r="O265" s="28" t="s">
         <v>828</v>
       </c>
       <c r="P265" s="28" t="s">
-        <v>1099</v>
+        <v>1084</v>
       </c>
       <c r="Q265" s="28" t="s">
         <v>826</v>
       </c>
       <c r="R265" s="29"/>
       <c r="S265" s="30" t="s">
-        <v>925</v>
+        <v>913</v>
       </c>
       <c r="T265" s="31" t="s">
         <v>51</v>
@@ -18403,13 +18414,13 @@
         <v>45013</v>
       </c>
       <c r="G266" s="27" t="s">
-        <v>941</v>
+        <v>929</v>
       </c>
       <c r="H266" s="27" t="s">
-        <v>942</v>
+        <v>930</v>
       </c>
       <c r="I266" s="27" t="s">
-        <v>943</v>
+        <v>931</v>
       </c>
       <c r="J266" s="28" t="s">
         <v>488</v>
@@ -18422,26 +18433,26 @@
         <v>828</v>
       </c>
       <c r="N266" s="28" t="s">
-        <v>1098</v>
+        <v>1083</v>
       </c>
       <c r="O266" s="28" t="s">
         <v>828</v>
       </c>
       <c r="P266" s="28" t="s">
-        <v>1099</v>
+        <v>1084</v>
       </c>
       <c r="Q266" s="28" t="s">
         <v>826</v>
       </c>
       <c r="R266" s="29"/>
       <c r="S266" s="30" t="s">
-        <v>925</v>
+        <v>913</v>
       </c>
       <c r="T266" s="31" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="267" spans="1:20" ht="116.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="267" spans="1:20" ht="131" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A267" s="23">
         <v>236</v>
       </c>
@@ -18461,13 +18472,13 @@
         <v>45012</v>
       </c>
       <c r="G267" s="27" t="s">
-        <v>926</v>
+        <v>914</v>
       </c>
       <c r="H267" s="27" t="s">
-        <v>928</v>
+        <v>916</v>
       </c>
       <c r="I267" s="27" t="s">
-        <v>860</v>
+        <v>848</v>
       </c>
       <c r="J267" s="28" t="s">
         <v>488</v>
@@ -18480,13 +18491,13 @@
         <v>488</v>
       </c>
       <c r="N267" s="28" t="s">
-        <v>929</v>
+        <v>917</v>
       </c>
       <c r="O267" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P267" s="28" t="s">
-        <v>1072</v>
+        <v>1057</v>
       </c>
       <c r="Q267" s="28" t="s">
         <v>826</v>
@@ -18517,13 +18528,13 @@
         <v>45022</v>
       </c>
       <c r="G268" s="27" t="s">
-        <v>1080</v>
+        <v>1065</v>
       </c>
       <c r="H268" s="34" t="s">
-        <v>1081</v>
+        <v>1066</v>
       </c>
       <c r="I268" s="27" t="s">
-        <v>860</v>
+        <v>848</v>
       </c>
       <c r="J268" s="28" t="s">
         <v>488</v>
@@ -18536,13 +18547,13 @@
         <v>488</v>
       </c>
       <c r="N268" s="28" t="s">
-        <v>929</v>
+        <v>917</v>
       </c>
       <c r="O268" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P268" s="28" t="s">
-        <v>1079</v>
+        <v>1064</v>
       </c>
       <c r="Q268" s="28" t="s">
         <v>826</v>
@@ -18553,7 +18564,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="269" spans="1:20" ht="232.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="269" spans="1:20" ht="261.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A269" s="23">
         <v>238</v>
       </c>
@@ -18573,13 +18584,13 @@
         <v>45035</v>
       </c>
       <c r="G269" s="27" t="s">
-        <v>1110</v>
+        <v>1095</v>
       </c>
       <c r="H269" s="34" t="s">
-        <v>1111</v>
+        <v>1096</v>
       </c>
       <c r="I269" s="27" t="s">
-        <v>860</v>
+        <v>848</v>
       </c>
       <c r="J269" s="28" t="s">
         <v>488</v>
@@ -18592,13 +18603,13 @@
         <v>488</v>
       </c>
       <c r="N269" s="28" t="s">
-        <v>1112</v>
+        <v>1097</v>
       </c>
       <c r="O269" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P269" s="28" t="s">
-        <v>1090</v>
+        <v>1075</v>
       </c>
       <c r="Q269" s="28" t="s">
         <v>826</v>
@@ -18629,13 +18640,13 @@
         <v>45023</v>
       </c>
       <c r="G270" s="27" t="s">
-        <v>1082</v>
+        <v>1067</v>
       </c>
       <c r="H270" s="34" t="s">
-        <v>1083</v>
+        <v>1068</v>
       </c>
       <c r="I270" s="27" t="s">
-        <v>860</v>
+        <v>848</v>
       </c>
       <c r="J270" s="28" t="s">
         <v>488</v>
@@ -18648,13 +18659,13 @@
         <v>488</v>
       </c>
       <c r="N270" s="28" t="s">
-        <v>929</v>
+        <v>917</v>
       </c>
       <c r="O270" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P270" s="28" t="s">
-        <v>1084</v>
+        <v>1069</v>
       </c>
       <c r="Q270" s="28" t="s">
         <v>826</v>
@@ -18685,13 +18696,13 @@
         <v>45012</v>
       </c>
       <c r="G271" s="27" t="s">
-        <v>930</v>
+        <v>918</v>
       </c>
       <c r="H271" s="27" t="s">
-        <v>931</v>
+        <v>919</v>
       </c>
       <c r="I271" s="27" t="s">
-        <v>860</v>
+        <v>848</v>
       </c>
       <c r="J271" s="28" t="s">
         <v>488</v>
@@ -18704,13 +18715,13 @@
         <v>488</v>
       </c>
       <c r="N271" s="28" t="s">
-        <v>932</v>
+        <v>920</v>
       </c>
       <c r="O271" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P271" s="28" t="s">
-        <v>1079</v>
+        <v>1064</v>
       </c>
       <c r="Q271" s="28" t="s">
         <v>826</v>
@@ -18741,13 +18752,13 @@
         <v>45023</v>
       </c>
       <c r="G272" s="27" t="s">
-        <v>1085</v>
+        <v>1070</v>
       </c>
       <c r="H272" s="27" t="s">
-        <v>1086</v>
+        <v>1071</v>
       </c>
       <c r="I272" s="27" t="s">
-        <v>860</v>
+        <v>848</v>
       </c>
       <c r="J272" s="28" t="s">
         <v>488</v>
@@ -18760,13 +18771,13 @@
         <v>488</v>
       </c>
       <c r="N272" s="28" t="s">
-        <v>1028</v>
+        <v>1016</v>
       </c>
       <c r="O272" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P272" s="28" t="s">
-        <v>1087</v>
+        <v>1072</v>
       </c>
       <c r="Q272" s="28" t="s">
         <v>826</v>
@@ -18777,7 +18788,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="273" spans="1:20" ht="189" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="273" spans="1:20" ht="203.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A273" s="23">
         <v>330</v>
       </c>
@@ -18797,13 +18808,13 @@
         <v>45027</v>
       </c>
       <c r="G273" s="27" t="s">
-        <v>1091</v>
+        <v>1076</v>
       </c>
       <c r="H273" s="43" t="s">
-        <v>1092</v>
+        <v>1077</v>
       </c>
       <c r="I273" s="27" t="s">
-        <v>860</v>
+        <v>848</v>
       </c>
       <c r="J273" s="28" t="s">
         <v>488</v>
@@ -18816,13 +18827,13 @@
         <v>488</v>
       </c>
       <c r="N273" s="28" t="s">
-        <v>1093</v>
+        <v>1078</v>
       </c>
       <c r="O273" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P273" s="28" t="s">
-        <v>1079</v>
+        <v>1064</v>
       </c>
       <c r="Q273" s="28" t="s">
         <v>826</v>
@@ -18833,7 +18844,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="274" spans="1:20" ht="218" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="274" spans="1:20" ht="232.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A274" s="23">
         <v>331</v>
       </c>
@@ -18853,13 +18864,13 @@
         <v>45023</v>
       </c>
       <c r="G274" s="27" t="s">
-        <v>1088</v>
+        <v>1073</v>
       </c>
       <c r="H274" s="27" t="s">
-        <v>1089</v>
+        <v>1074</v>
       </c>
       <c r="I274" s="27" t="s">
-        <v>860</v>
+        <v>848</v>
       </c>
       <c r="J274" s="28" t="s">
         <v>488</v>
@@ -18872,13 +18883,13 @@
         <v>488</v>
       </c>
       <c r="N274" s="28" t="s">
-        <v>1028</v>
+        <v>1016</v>
       </c>
       <c r="O274" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P274" s="28" t="s">
-        <v>1090</v>
+        <v>1075</v>
       </c>
       <c r="Q274" s="28" t="s">
         <v>826</v>
@@ -18909,13 +18920,13 @@
         <v>45033</v>
       </c>
       <c r="G275" s="27" t="s">
-        <v>1102</v>
+        <v>1087</v>
       </c>
       <c r="H275" s="34" t="s">
-        <v>1103</v>
+        <v>1088</v>
       </c>
       <c r="I275" s="27" t="s">
-        <v>860</v>
+        <v>848</v>
       </c>
       <c r="J275" s="28" t="s">
         <v>488</v>
@@ -18928,13 +18939,13 @@
         <v>488</v>
       </c>
       <c r="N275" s="28" t="s">
-        <v>1104</v>
+        <v>1089</v>
       </c>
       <c r="O275" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P275" s="28" t="s">
-        <v>1079</v>
+        <v>1064</v>
       </c>
       <c r="Q275" s="28" t="s">
         <v>826</v>
@@ -18965,13 +18976,13 @@
         <v>45031</v>
       </c>
       <c r="G276" s="27" t="s">
-        <v>1100</v>
+        <v>1085</v>
       </c>
       <c r="H276" s="34" t="s">
-        <v>1101</v>
+        <v>1086</v>
       </c>
       <c r="I276" s="27" t="s">
-        <v>860</v>
+        <v>848</v>
       </c>
       <c r="J276" s="28" t="s">
         <v>488</v>
@@ -18984,13 +18995,13 @@
         <v>488</v>
       </c>
       <c r="N276" s="28" t="s">
-        <v>1028</v>
+        <v>1016</v>
       </c>
       <c r="O276" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P276" s="28" t="s">
-        <v>1079</v>
+        <v>1064</v>
       </c>
       <c r="Q276" s="28" t="s">
         <v>826</v>
@@ -20820,16 +20831,16 @@
         <v>687</v>
       </c>
       <c r="F330" s="26">
-        <v>45013</v>
+        <v>45055</v>
       </c>
       <c r="G330" s="27" t="s">
-        <v>1061</v>
+        <v>1115</v>
       </c>
       <c r="H330" s="27" t="s">
-        <v>1062</v>
+        <v>1116</v>
       </c>
       <c r="I330" s="27" t="s">
-        <v>1063</v>
+        <v>1117</v>
       </c>
       <c r="J330" s="28" t="s">
         <v>488</v>
@@ -20873,7 +20884,7 @@
         <v>828</v>
       </c>
       <c r="K331" s="28" t="s">
-        <v>1064</v>
+        <v>1049</v>
       </c>
       <c r="L331" s="28"/>
       <c r="M331" s="28"/>
@@ -20911,7 +20922,7 @@
         <v>828</v>
       </c>
       <c r="K332" s="28" t="s">
-        <v>1065</v>
+        <v>1050</v>
       </c>
       <c r="L332" s="28"/>
       <c r="M332" s="28"/>
@@ -20949,7 +20960,7 @@
         <v>828</v>
       </c>
       <c r="K333" s="28" t="s">
-        <v>1066</v>
+        <v>1051</v>
       </c>
       <c r="L333" s="28"/>
       <c r="M333" s="28"/>
@@ -20983,13 +20994,13 @@
         <v>45013</v>
       </c>
       <c r="G334" s="27" t="s">
-        <v>948</v>
+        <v>936</v>
       </c>
       <c r="H334" s="37" t="s">
-        <v>949</v>
+        <v>937</v>
       </c>
       <c r="I334" s="27" t="s">
-        <v>950</v>
+        <v>938</v>
       </c>
       <c r="J334" s="28" t="s">
         <v>488</v>
@@ -21002,13 +21013,13 @@
         <v>488</v>
       </c>
       <c r="N334" s="28" t="s">
-        <v>951</v>
+        <v>939</v>
       </c>
       <c r="O334" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P334" s="28" t="s">
-        <v>1087</v>
+        <v>1072</v>
       </c>
       <c r="Q334" s="28" t="s">
         <v>826</v>
@@ -21039,13 +21050,13 @@
         <v>45013</v>
       </c>
       <c r="G335" s="27" t="s">
-        <v>944</v>
+        <v>932</v>
       </c>
       <c r="H335" s="27" t="s">
-        <v>945</v>
+        <v>933</v>
       </c>
       <c r="I335" s="27" t="s">
-        <v>946</v>
+        <v>934</v>
       </c>
       <c r="J335" s="28" t="s">
         <v>488</v>
@@ -21058,13 +21069,13 @@
         <v>488</v>
       </c>
       <c r="N335" s="28" t="s">
-        <v>947</v>
+        <v>935</v>
       </c>
       <c r="O335" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P335" s="28" t="s">
-        <v>1087</v>
+        <v>1072</v>
       </c>
       <c r="Q335" s="28" t="s">
         <v>826</v>
@@ -21095,13 +21106,13 @@
         <v>45013</v>
       </c>
       <c r="G336" s="27" t="s">
-        <v>952</v>
+        <v>940</v>
       </c>
       <c r="H336" s="27" t="s">
-        <v>953</v>
+        <v>941</v>
       </c>
       <c r="I336" s="27" t="s">
-        <v>955</v>
+        <v>943</v>
       </c>
       <c r="J336" s="28" t="s">
         <v>488</v>
@@ -21114,13 +21125,13 @@
         <v>488</v>
       </c>
       <c r="N336" s="28" t="s">
-        <v>954</v>
+        <v>942</v>
       </c>
       <c r="O336" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P336" s="28" t="s">
-        <v>1087</v>
+        <v>1072</v>
       </c>
       <c r="Q336" s="28" t="s">
         <v>826</v>
@@ -21151,13 +21162,13 @@
         <v>45013</v>
       </c>
       <c r="G337" s="27" t="s">
-        <v>956</v>
+        <v>944</v>
       </c>
       <c r="H337" s="27" t="s">
-        <v>957</v>
+        <v>945</v>
       </c>
       <c r="I337" s="27" t="s">
-        <v>958</v>
+        <v>946</v>
       </c>
       <c r="J337" s="28" t="s">
         <v>488</v>
@@ -21170,13 +21181,13 @@
         <v>488</v>
       </c>
       <c r="N337" s="28" t="s">
-        <v>959</v>
+        <v>947</v>
       </c>
       <c r="O337" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P337" s="28" t="s">
-        <v>1087</v>
+        <v>1072</v>
       </c>
       <c r="Q337" s="28" t="s">
         <v>826</v>
@@ -21207,13 +21218,13 @@
         <v>45013</v>
       </c>
       <c r="G338" s="27" t="s">
-        <v>960</v>
+        <v>948</v>
       </c>
       <c r="H338" s="27" t="s">
-        <v>961</v>
+        <v>949</v>
       </c>
       <c r="I338" s="27" t="s">
-        <v>962</v>
+        <v>950</v>
       </c>
       <c r="J338" s="28" t="s">
         <v>488</v>
@@ -21226,13 +21237,13 @@
         <v>488</v>
       </c>
       <c r="N338" s="28" t="s">
-        <v>963</v>
+        <v>951</v>
       </c>
       <c r="O338" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P338" s="28" t="s">
-        <v>1087</v>
+        <v>1072</v>
       </c>
       <c r="Q338" s="28" t="s">
         <v>826</v>
@@ -21263,13 +21274,13 @@
         <v>45013</v>
       </c>
       <c r="G339" s="27" t="s">
-        <v>964</v>
+        <v>952</v>
       </c>
       <c r="H339" s="27" t="s">
-        <v>965</v>
+        <v>953</v>
       </c>
       <c r="I339" s="27" t="s">
-        <v>966</v>
+        <v>954</v>
       </c>
       <c r="J339" s="28" t="s">
         <v>488</v>
@@ -21282,13 +21293,13 @@
         <v>488</v>
       </c>
       <c r="N339" s="28" t="s">
-        <v>967</v>
+        <v>955</v>
       </c>
       <c r="O339" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P339" s="28" t="s">
-        <v>1087</v>
+        <v>1072</v>
       </c>
       <c r="Q339" s="28" t="s">
         <v>826</v>
@@ -21323,7 +21334,7 @@
         <v>828</v>
       </c>
       <c r="K340" s="32" t="s">
-        <v>870</v>
+        <v>858</v>
       </c>
       <c r="L340" s="28"/>
       <c r="M340" s="28"/>
@@ -21357,13 +21368,13 @@
         <v>45014</v>
       </c>
       <c r="G341" s="27" t="s">
-        <v>968</v>
+        <v>956</v>
       </c>
       <c r="H341" s="27" t="s">
-        <v>969</v>
+        <v>957</v>
       </c>
       <c r="I341" s="27" t="s">
-        <v>970</v>
+        <v>958</v>
       </c>
       <c r="J341" s="28" t="s">
         <v>488</v>
@@ -21376,13 +21387,13 @@
         <v>488</v>
       </c>
       <c r="N341" s="28" t="s">
-        <v>971</v>
+        <v>959</v>
       </c>
       <c r="O341" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P341" s="28" t="s">
-        <v>1087</v>
+        <v>1072</v>
       </c>
       <c r="Q341" s="28" t="s">
         <v>826</v>
@@ -21413,13 +21424,13 @@
         <v>45014</v>
       </c>
       <c r="G342" s="27" t="s">
-        <v>972</v>
+        <v>960</v>
       </c>
       <c r="H342" s="27" t="s">
-        <v>973</v>
+        <v>961</v>
       </c>
       <c r="I342" s="27" t="s">
-        <v>974</v>
+        <v>962</v>
       </c>
       <c r="J342" s="28" t="s">
         <v>488</v>
@@ -21432,13 +21443,13 @@
         <v>488</v>
       </c>
       <c r="N342" s="28" t="s">
-        <v>975</v>
+        <v>963</v>
       </c>
       <c r="O342" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P342" s="28" t="s">
-        <v>1087</v>
+        <v>1072</v>
       </c>
       <c r="Q342" s="28" t="s">
         <v>826</v>
@@ -21449,7 +21460,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="343" spans="1:20" s="21" customFormat="1" ht="102" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="343" spans="1:20" s="21" customFormat="1" ht="116.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A343" s="23">
         <v>160</v>
       </c>
@@ -21469,13 +21480,13 @@
         <v>45014</v>
       </c>
       <c r="G343" s="27" t="s">
-        <v>977</v>
+        <v>965</v>
       </c>
       <c r="H343" s="27" t="s">
-        <v>978</v>
+        <v>966</v>
       </c>
       <c r="I343" s="27" t="s">
-        <v>979</v>
+        <v>967</v>
       </c>
       <c r="J343" s="28" t="s">
         <v>488</v>
@@ -21488,13 +21499,13 @@
         <v>488</v>
       </c>
       <c r="N343" s="28" t="s">
-        <v>976</v>
+        <v>964</v>
       </c>
       <c r="O343" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P343" s="28" t="s">
-        <v>1087</v>
+        <v>1072</v>
       </c>
       <c r="Q343" s="28" t="s">
         <v>826</v>
@@ -21525,13 +21536,13 @@
         <v>45014</v>
       </c>
       <c r="G344" s="27" t="s">
-        <v>982</v>
+        <v>970</v>
       </c>
       <c r="H344" s="27" t="s">
-        <v>981</v>
+        <v>969</v>
       </c>
       <c r="I344" s="27" t="s">
-        <v>980</v>
+        <v>968</v>
       </c>
       <c r="J344" s="28" t="s">
         <v>488</v>
@@ -21544,13 +21555,13 @@
         <v>488</v>
       </c>
       <c r="N344" s="28" t="s">
-        <v>983</v>
+        <v>971</v>
       </c>
       <c r="O344" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P344" s="28" t="s">
-        <v>1087</v>
+        <v>1072</v>
       </c>
       <c r="Q344" s="28" t="s">
         <v>826</v>
@@ -21581,13 +21592,13 @@
         <v>45014</v>
       </c>
       <c r="G345" s="27" t="s">
-        <v>984</v>
+        <v>972</v>
       </c>
       <c r="H345" s="27" t="s">
-        <v>985</v>
+        <v>973</v>
       </c>
       <c r="I345" s="27" t="s">
-        <v>986</v>
+        <v>974</v>
       </c>
       <c r="J345" s="28" t="s">
         <v>488</v>
@@ -21600,13 +21611,13 @@
         <v>488</v>
       </c>
       <c r="N345" s="28" t="s">
-        <v>987</v>
+        <v>975</v>
       </c>
       <c r="O345" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P345" s="28" t="s">
-        <v>1087</v>
+        <v>1072</v>
       </c>
       <c r="Q345" s="28" t="s">
         <v>826</v>
@@ -21641,7 +21652,7 @@
         <v>828</v>
       </c>
       <c r="K346" s="28" t="s">
-        <v>988</v>
+        <v>976</v>
       </c>
       <c r="L346" s="28"/>
       <c r="M346" s="28"/>
@@ -21679,7 +21690,7 @@
         <v>828</v>
       </c>
       <c r="K347" s="28" t="s">
-        <v>934</v>
+        <v>922</v>
       </c>
       <c r="L347" s="28"/>
       <c r="M347" s="28"/>
@@ -21717,7 +21728,7 @@
         <v>828</v>
       </c>
       <c r="K348" s="28" t="s">
-        <v>934</v>
+        <v>922</v>
       </c>
       <c r="L348" s="28"/>
       <c r="M348" s="28"/>
@@ -21755,7 +21766,7 @@
         <v>828</v>
       </c>
       <c r="K349" s="28" t="s">
-        <v>934</v>
+        <v>922</v>
       </c>
       <c r="L349" s="28"/>
       <c r="M349" s="28"/>
@@ -21793,7 +21804,7 @@
         <v>828</v>
       </c>
       <c r="K350" s="28" t="s">
-        <v>934</v>
+        <v>922</v>
       </c>
       <c r="L350" s="28"/>
       <c r="M350" s="28"/>
@@ -21827,13 +21838,13 @@
         <v>45014</v>
       </c>
       <c r="G351" s="27" t="s">
-        <v>990</v>
+        <v>978</v>
       </c>
       <c r="H351" s="26" t="s">
-        <v>991</v>
+        <v>979</v>
       </c>
       <c r="I351" s="26" t="s">
-        <v>989</v>
+        <v>977</v>
       </c>
       <c r="J351" s="26" t="s">
         <v>488</v>
@@ -21846,13 +21857,13 @@
         <v>488</v>
       </c>
       <c r="N351" s="26" t="s">
-        <v>992</v>
+        <v>980</v>
       </c>
       <c r="O351" s="28" t="s">
         <v>488</v>
       </c>
       <c r="P351" s="28" t="s">
-        <v>1087</v>
+        <v>1072</v>
       </c>
       <c r="Q351" s="28" t="s">
         <v>826</v>
@@ -21883,13 +21894,13 @@
         <v>45014</v>
       </c>
       <c r="G352" s="26" t="s">
-        <v>993</v>
+        <v>981</v>
       </c>
       <c r="H352" s="26" t="s">
-        <v>994</v>
+        <v>982</v>
       </c>
       <c r="I352" s="26" t="s">
-        <v>995</v>
+        <v>983</v>
       </c>
       <c r="J352" s="26" t="s">
         <v>488</v>
@@ -21902,13 +21913,13 @@
         <v>488</v>
       </c>
       <c r="N352" s="26" t="s">
-        <v>996</v>
+        <v>984</v>
       </c>
       <c r="O352" s="26" t="s">
         <v>488</v>
       </c>
       <c r="P352" s="26" t="s">
-        <v>1087</v>
+        <v>1072</v>
       </c>
       <c r="Q352" s="26" t="s">
         <v>826</v>

</xml_diff>

<commit_message>
Aggiornamento file per mancato accreditamento
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111SYNLABXXXXX/Synlab_SDN/Sdn.Net/1.1.0.0/accreditamento-checklist_V8.1.2.xlsx
+++ b/GATEWAY/A1#111SYNLABXXXXX/Synlab_SDN/Sdn.Net/1.1.0.0/accreditamento-checklist_V8.1.2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.1.163\D_Drive\tmp\RepositoryFSE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A2AD1C-7685-4AE9-8EDD-2D8265C423D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D771290-0E6E-4B78-870D-C8997BC01C92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -5337,22 +5337,22 @@
     <t>2.16.840.1.113883.2.9.2.150.4.4.4c33ed9800b3a644e5dba5c93b19657747d608f82ee2f9e7440000d729dacf88.5dca9c7cf3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2023-05-11T12:27:45Z</t>
-  </si>
-  <si>
-    <t>576f5986cf24105c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.7187842f4612b0625de53a51e8eb67fb300bc0db749ea1c0461a6715ea1d9bee.058cfd2e07^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-05-11T14:50:51Z</t>
-  </si>
-  <si>
-    <t>9dda526eec565c69</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.e110c92e94948a859dd64ae68f72e73e512046f9d0241b82496a0b8d154e6a8e.3ed2463a91^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-05-16T09:53:45Z</t>
+  </si>
+  <si>
+    <t>18af7c9d63a24a25</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.9ce9bf2e676693602146930bed6a6a988a61c28fa054aedff11202395c09fc44.34eff48263^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-05-16T09:59:36Z</t>
+  </si>
+  <si>
+    <t>3330bf287d3a27eb</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.3feb80e08f25a65b3bea91355a75c064b7f4ed00f3708cf96b622bf201eb4272.b25096cfae^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -8780,7 +8780,7 @@
         <v>426</v>
       </c>
       <c r="F15" s="26">
-        <v>45057</v>
+        <v>45062</v>
       </c>
       <c r="G15" s="27" t="s">
         <v>1112</v>
@@ -8813,7 +8813,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="232.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:20" ht="247" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="23">
         <v>242</v>
       </c>
@@ -8847,7 +8847,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="218" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:20" ht="232.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="23">
         <v>253</v>
       </c>
@@ -8881,7 +8881,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="232.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:20" ht="247" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="23">
         <v>258</v>
       </c>
@@ -8915,7 +8915,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="218" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:20" ht="232.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="23">
         <v>269</v>
       </c>
@@ -9403,7 +9403,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="174.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:20" ht="189" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="23">
         <v>358</v>
       </c>
@@ -9439,7 +9439,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="203.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:20" ht="218" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="23">
         <v>359</v>
       </c>
@@ -9475,7 +9475,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="174.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:20" ht="189" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="23">
         <v>360</v>
       </c>
@@ -9509,7 +9509,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="203.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:20" ht="218" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="23">
         <v>361</v>
       </c>
@@ -9825,7 +9825,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="116.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:20" ht="131" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="23">
         <v>204</v>
       </c>
@@ -9893,7 +9893,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="116.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:20" ht="131" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="23">
         <v>220</v>
       </c>
@@ -10073,7 +10073,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="116.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:20" ht="131" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="23">
         <v>252</v>
       </c>
@@ -10141,7 +10141,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="116.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:20" ht="131" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51" s="23">
         <v>268</v>
       </c>
@@ -10209,7 +10209,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="116.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:20" ht="131" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="23">
         <v>284</v>
       </c>
@@ -10289,7 +10289,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="116.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:20" ht="131" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" s="23">
         <v>300</v>
       </c>
@@ -10379,7 +10379,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="116.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:20" ht="131" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A57" s="23">
         <v>316</v>
       </c>
@@ -11223,7 +11223,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="80" spans="1:20" ht="189" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:20" ht="203.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A80" s="23">
         <v>202</v>
       </c>
@@ -11291,7 +11291,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="82" spans="1:20" ht="160" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:20" ht="174.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A82" s="23">
         <v>208</v>
       </c>
@@ -11495,7 +11495,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="88" spans="1:20" ht="189" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:20" ht="203.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A88" s="23">
         <v>218</v>
       </c>
@@ -11619,7 +11619,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="91" spans="1:20" ht="160" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:20" ht="174.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A91" s="23">
         <v>77</v>
       </c>
@@ -12197,7 +12197,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="104" spans="1:20" ht="203.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:20" ht="218" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A104" s="23">
         <v>250</v>
       </c>
@@ -12469,7 +12469,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="112" spans="1:20" ht="203.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:20" ht="218" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A112" s="23">
         <v>266</v>
       </c>
@@ -12741,7 +12741,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="120" spans="1:20" ht="189" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:20" ht="203.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A120" s="23">
         <v>282</v>
       </c>
@@ -12809,7 +12809,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="122" spans="1:20" ht="160" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="122" spans="1:20" ht="174.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A122" s="23">
         <v>288</v>
       </c>
@@ -13137,7 +13137,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="128" spans="1:20" ht="189" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="128" spans="1:20" ht="203.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A128" s="23">
         <v>298</v>
       </c>
@@ -13453,7 +13453,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="136" spans="1:20" ht="189" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="136" spans="1:20" ht="203.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A136" s="23">
         <v>314</v>
       </c>
@@ -14153,7 +14153,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="154" spans="1:20" ht="247" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="154" spans="1:20" ht="261.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A154" s="23">
         <v>193</v>
       </c>
@@ -14187,7 +14187,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="155" spans="1:20" ht="247" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="155" spans="1:20" ht="276" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A155" s="23">
         <v>206</v>
       </c>
@@ -14221,7 +14221,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="156" spans="1:20" ht="247" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="156" spans="1:20" ht="261.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A156" s="23">
         <v>209</v>
       </c>
@@ -14255,7 +14255,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="157" spans="1:20" ht="232.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="157" spans="1:20" ht="261.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A157" s="23">
         <v>222</v>
       </c>
@@ -14365,7 +14365,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="160" spans="1:20" ht="261.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="160" spans="1:20" ht="290.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A160" s="23">
         <v>241</v>
       </c>
@@ -14399,7 +14399,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="161" spans="1:20" ht="247" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="161" spans="1:20" ht="276" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A161" s="23">
         <v>254</v>
       </c>
@@ -14433,7 +14433,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="162" spans="1:20" ht="261.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="162" spans="1:20" ht="290.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A162" s="23">
         <v>257</v>
       </c>
@@ -14467,7 +14467,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="163" spans="1:20" ht="247" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="163" spans="1:20" ht="276" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A163" s="23">
         <v>270</v>
       </c>
@@ -14501,7 +14501,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="164" spans="1:20" ht="247" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="164" spans="1:20" ht="261.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A164" s="23">
         <v>273</v>
       </c>
@@ -14535,7 +14535,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="165" spans="1:20" ht="232.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="165" spans="1:20" ht="261.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A165" s="23">
         <v>286</v>
       </c>
@@ -14569,7 +14569,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="166" spans="1:20" ht="247" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="166" spans="1:20" ht="261.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A166" s="23">
         <v>289</v>
       </c>
@@ -14621,7 +14621,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="167" spans="1:20" ht="232.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="167" spans="1:20" ht="261.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A167" s="23">
         <v>302</v>
       </c>
@@ -14677,7 +14677,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="168" spans="1:20" ht="247" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="168" spans="1:20" ht="261.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A168" s="23">
         <v>305</v>
       </c>
@@ -14711,7 +14711,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="169" spans="1:20" ht="232.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="169" spans="1:20" ht="261.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A169" s="23">
         <v>318</v>
       </c>
@@ -14745,7 +14745,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="170" spans="1:20" ht="189" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="170" spans="1:20" ht="203.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A170" s="23">
         <v>322</v>
       </c>
@@ -14779,7 +14779,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="171" spans="1:20" ht="218" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="171" spans="1:20" ht="232.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A171" s="23">
         <v>323</v>
       </c>
@@ -14813,7 +14813,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="172" spans="1:20" ht="189" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="172" spans="1:20" ht="203.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A172" s="23">
         <v>326</v>
       </c>
@@ -14847,7 +14847,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="173" spans="1:20" ht="218" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="173" spans="1:20" ht="232.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A173" s="23">
         <v>327</v>
       </c>
@@ -14957,7 +14957,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="176" spans="1:20" ht="189" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="176" spans="1:20" ht="203.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A176" s="23">
         <v>334</v>
       </c>
@@ -14991,7 +14991,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="177" spans="1:20" ht="232.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="177" spans="1:20" ht="247" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A177" s="23">
         <v>335</v>
       </c>
@@ -15025,7 +15025,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="178" spans="1:20" ht="203.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="178" spans="1:20" ht="218" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A178" s="23">
         <v>338</v>
       </c>
@@ -15059,7 +15059,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="179" spans="1:20" ht="232.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="179" spans="1:20" ht="247" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A179" s="23">
         <v>339</v>
       </c>
@@ -15093,7 +15093,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="180" spans="1:20" ht="189" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="180" spans="1:20" ht="203.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A180" s="23">
         <v>342</v>
       </c>
@@ -15127,7 +15127,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="181" spans="1:20" ht="218" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="181" spans="1:20" ht="232.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A181" s="23">
         <v>343</v>
       </c>
@@ -15161,7 +15161,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="182" spans="1:20" ht="174.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="182" spans="1:20" ht="189" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A182" s="23">
         <v>346</v>
       </c>
@@ -15217,7 +15217,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="183" spans="1:20" ht="218" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="183" spans="1:20" ht="232.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A183" s="23">
         <v>347</v>
       </c>
@@ -15275,7 +15275,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="184" spans="1:20" ht="189" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="184" spans="1:20" ht="203.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A184" s="23">
         <v>350</v>
       </c>
@@ -15309,7 +15309,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="185" spans="1:20" ht="218" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="185" spans="1:20" ht="232.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A185" s="23">
         <v>351</v>
       </c>
@@ -16347,7 +16347,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="214" spans="1:20" ht="160" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="214" spans="1:20" ht="174.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A214" s="23">
         <v>224</v>
       </c>
@@ -16657,7 +16657,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="222" spans="1:20" ht="247" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="222" spans="1:20" ht="261.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A222" s="23">
         <v>225</v>
       </c>
@@ -18336,7 +18336,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="265" spans="1:20" ht="189" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="265" spans="1:20" ht="203.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A265" s="23">
         <v>234</v>
       </c>
@@ -18452,7 +18452,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="267" spans="1:20" ht="116.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="267" spans="1:20" ht="131" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A267" s="23">
         <v>236</v>
       </c>
@@ -18564,7 +18564,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="269" spans="1:20" ht="232.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="269" spans="1:20" ht="261.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A269" s="23">
         <v>238</v>
       </c>
@@ -18788,7 +18788,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="273" spans="1:20" ht="189" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="273" spans="1:20" ht="203.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A273" s="23">
         <v>330</v>
       </c>
@@ -18844,7 +18844,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="274" spans="1:20" ht="218" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="274" spans="1:20" ht="232.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A274" s="23">
         <v>331</v>
       </c>
@@ -20831,7 +20831,7 @@
         <v>687</v>
       </c>
       <c r="F330" s="26">
-        <v>45057</v>
+        <v>45062</v>
       </c>
       <c r="G330" s="27" t="s">
         <v>1115</v>
@@ -21460,7 +21460,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="343" spans="1:20" s="21" customFormat="1" ht="102" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="343" spans="1:20" s="21" customFormat="1" ht="116.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A343" s="23">
         <v>160</v>
       </c>

</xml_diff>